<commit_message>
updated mendeley some more
</commit_message>
<xml_diff>
--- a/temp_table.xlsx
+++ b/temp_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buchanan/OneDrive - Missouri State University/RESEARCH/2 projects/Table-of-Doom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6631179C-32FD-634A-8AF2-815A44C206B1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D8FE969D-235A-6049-A0EE-B1053071954A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14500" xr2:uid="{DAE7CE15-139C-094D-A13B-3BB5233284F4}"/>
   </bookViews>
@@ -1696,15 +1696,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -2026,8 +2018,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="A8:E10"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
+      <selection activeCell="E39" sqref="A36:E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.83203125" defaultRowHeight="16"/>
@@ -2223,53 +2215,53 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="64">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="1">
-        <v>2014</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B12" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="96">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="2">
         <v>2011</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="64">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="2">
         <v>2010</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2330,19 +2322,19 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="80">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="2">
         <v>2009</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="2" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2406,87 +2398,87 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="80">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24" s="2">
         <v>2010</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E24" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="48">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="1">
-        <v>2014</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="B25" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="1" t="s">
+      <c r="D25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="48">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B26" s="1">
-        <v>2014</v>
-      </c>
-      <c r="C26" s="1" t="s">
+      <c r="B26" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" s="1" t="s">
+      <c r="D26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="48">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B27" s="1">
-        <v>2014</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="B27" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" s="1" t="s">
+      <c r="D27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="64">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="2">
         <v>2008</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="1" t="s">
+      <c r="D28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2502,172 +2494,172 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="64">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B30" s="1">
-        <v>2014</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="B30" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E30" s="1" t="s">
+      <c r="D30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="80">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B31" s="1">
-        <v>2014</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="B31" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E31" s="1" t="s">
+      <c r="D31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="48">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="2">
         <v>2003</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" s="2" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="128">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="2">
         <v>2000</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="2" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="48">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34" s="2">
         <v>1994</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" s="2" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="96">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B35" s="1">
-        <v>2014</v>
-      </c>
-      <c r="C35" s="1" t="s">
+      <c r="B35" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E35" s="1" t="s">
+      <c r="D35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="80">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B36" s="1">
-        <v>2014</v>
-      </c>
-      <c r="C36" s="1" t="s">
+      <c r="B36" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E36" s="1" t="s">
+      <c r="D36" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="64">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="2">
         <v>2004</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E37" s="2" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="48">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B38" s="1">
-        <v>2014</v>
-      </c>
-      <c r="C38" s="1" t="s">
+      <c r="B38" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E38" s="1" t="s">
+      <c r="D38" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="32">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B39" s="1">
-        <v>2014</v>
-      </c>
-      <c r="C39" s="1" t="s">
+      <c r="B39" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E39" s="1" t="s">
+      <c r="D39" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>124</v>
       </c>
     </row>
@@ -4339,53 +4331,53 @@
       </c>
     </row>
     <row r="140" spans="1:5" ht="96">
-      <c r="A140" s="1" t="s">
+      <c r="A140" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="B140" s="1">
-        <v>2014</v>
-      </c>
-      <c r="C140" s="1" t="s">
+      <c r="B140" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C140" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="D140" s="1" t="s">
+      <c r="D140" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="E140" s="1" t="s">
+      <c r="E140" s="2" t="s">
         <v>435</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="96">
-      <c r="A141" s="1" t="s">
+      <c r="A141" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="B141" s="1">
+      <c r="B141" s="2">
         <v>2015</v>
       </c>
-      <c r="C141" s="1" t="s">
+      <c r="C141" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="D141" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E141" s="1" t="s">
+      <c r="D141" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E141" s="2" t="s">
         <v>438</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="96">
-      <c r="A142" s="1" t="s">
+      <c r="A142" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="B142" s="1">
+      <c r="B142" s="2">
         <v>2015</v>
       </c>
-      <c r="C142" s="1" t="s">
+      <c r="C142" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="D142" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E142" s="1" t="s">
+      <c r="D142" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E142" s="2" t="s">
         <v>441</v>
       </c>
     </row>
@@ -4404,19 +4396,19 @@
       </c>
     </row>
     <row r="144" spans="1:5" ht="48">
-      <c r="A144" s="1" t="s">
+      <c r="A144" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="B144" s="1">
-        <v>2014</v>
-      </c>
-      <c r="C144" s="1" t="s">
+      <c r="B144" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C144" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="D144" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E144" s="1" t="s">
+      <c r="D144" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E144" s="2" t="s">
         <v>447</v>
       </c>
     </row>
@@ -4449,53 +4441,53 @@
       </c>
     </row>
     <row r="147" spans="1:5" ht="48">
-      <c r="A147" s="1" t="s">
+      <c r="A147" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="B147" s="1">
-        <v>2014</v>
-      </c>
-      <c r="C147" s="1" t="s">
+      <c r="B147" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C147" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="D147" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E147" s="1" t="s">
+      <c r="D147" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E147" s="2" t="s">
         <v>456</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="96">
-      <c r="A148" s="1" t="s">
+      <c r="A148" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="B148" s="1">
+      <c r="B148" s="2">
         <v>2017</v>
       </c>
-      <c r="C148" s="1" t="s">
+      <c r="C148" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="D148" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E148" s="1" t="s">
+      <c r="D148" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E148" s="2" t="s">
         <v>459</v>
       </c>
     </row>
     <row r="149" spans="1:5" ht="48">
-      <c r="A149" s="1" t="s">
+      <c r="A149" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="B149" s="1">
+      <c r="B149" s="2">
         <v>2015</v>
       </c>
-      <c r="C149" s="1" t="s">
+      <c r="C149" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="D149" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E149" s="1" t="s">
+      <c r="D149" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E149" s="2" t="s">
         <v>462</v>
       </c>
     </row>
@@ -4892,7 +4884,7 @@
       </customFilters>
     </filterColumn>
     <sortState ref="A2:E172">
-      <sortCondition sortBy="cellColor" ref="E1:E172" dxfId="1"/>
+      <sortCondition sortBy="cellColor" ref="E1:E172" dxfId="0"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updating my mendeley stuff
</commit_message>
<xml_diff>
--- a/temp_table.xlsx
+++ b/temp_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/buchanan/OneDrive - Missouri State University/RESEARCH/2 projects/Table-of-Doom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D8FE969D-235A-6049-A0EE-B1053071954A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C370D80B-A121-8B45-A3C7-527969ECD5A2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14500" xr2:uid="{DAE7CE15-139C-094D-A13B-3BB5233284F4}"/>
+    <workbookView xWindow="-24080" yWindow="460" windowWidth="25040" windowHeight="13940" xr2:uid="{DAE7CE15-139C-094D-A13B-3BB5233284F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2015,11 +2015,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{805282B3-09CF-524D-BE5F-512790502F08}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:E172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
-      <selection activeCell="E39" sqref="A36:E39"/>
+    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
+      <selection activeCell="B117" sqref="B117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="30.83203125" defaultRowHeight="16"/>
@@ -2200,7 +2199,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="48" hidden="1">
+    <row r="11" spans="1:5" ht="48">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
@@ -2265,7 +2264,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="64" hidden="1">
+    <row r="15" spans="1:5" ht="64">
       <c r="A15" s="1" t="s">
         <v>46</v>
       </c>
@@ -2279,7 +2278,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="48" hidden="1">
+    <row r="16" spans="1:5" ht="48">
       <c r="A16" s="1" t="s">
         <v>49</v>
       </c>
@@ -2293,7 +2292,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="32" hidden="1">
+    <row r="17" spans="1:5" ht="32">
       <c r="A17" s="1" t="s">
         <v>52</v>
       </c>
@@ -2307,7 +2306,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="48" hidden="1">
+    <row r="18" spans="1:5" ht="48">
       <c r="A18" s="1" t="s">
         <v>55</v>
       </c>
@@ -2338,7 +2337,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="64" hidden="1">
+    <row r="20" spans="1:5" ht="64">
       <c r="A20" s="1" t="s">
         <v>62</v>
       </c>
@@ -2352,7 +2351,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="96" hidden="1">
+    <row r="21" spans="1:5" ht="96">
       <c r="A21" s="1" t="s">
         <v>64</v>
       </c>
@@ -2383,7 +2382,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="64" hidden="1">
+    <row r="23" spans="1:5" ht="64">
       <c r="A23" s="1" t="s">
         <v>71</v>
       </c>
@@ -2482,7 +2481,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="48" hidden="1">
+    <row r="29" spans="1:5" ht="48">
       <c r="A29" s="1" t="s">
         <v>90</v>
       </c>
@@ -2935,7 +2934,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="112" hidden="1">
+    <row r="56" spans="1:5" ht="112">
       <c r="A56" s="1" t="s">
         <v>173</v>
       </c>
@@ -3051,7 +3050,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="48" hidden="1">
+    <row r="63" spans="1:5" ht="48">
       <c r="A63" s="1" t="s">
         <v>196</v>
       </c>
@@ -3113,7 +3112,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="112" hidden="1">
+    <row r="67" spans="1:5" ht="112">
       <c r="A67" s="1" t="s">
         <v>208</v>
       </c>
@@ -3603,7 +3602,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="96" hidden="1">
+    <row r="96" spans="1:5" ht="96">
       <c r="A96" s="1" t="s">
         <v>303</v>
       </c>
@@ -3923,7 +3922,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="80" hidden="1">
+    <row r="115" spans="1:5" ht="80">
       <c r="A115" s="1" t="s">
         <v>359</v>
       </c>
@@ -3971,7 +3970,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="118" spans="1:5" hidden="1">
+    <row r="118" spans="1:5">
       <c r="A118" s="1" t="s">
         <v>368</v>
       </c>
@@ -4084,7 +4083,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="64" hidden="1">
+    <row r="125" spans="1:5" ht="64">
       <c r="A125" s="1" t="s">
         <v>389</v>
       </c>
@@ -4180,7 +4179,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="96" hidden="1">
+    <row r="131" spans="1:5" ht="96">
       <c r="A131" s="1" t="s">
         <v>405</v>
       </c>
@@ -4381,7 +4380,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="64" hidden="1">
+    <row r="143" spans="1:5" ht="64">
       <c r="A143" s="1" t="s">
         <v>442</v>
       </c>
@@ -4412,7 +4411,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="128" hidden="1">
+    <row r="145" spans="1:5" ht="128">
       <c r="A145" s="1" t="s">
         <v>448</v>
       </c>
@@ -4426,7 +4425,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="80" hidden="1">
+    <row r="146" spans="1:5" ht="80">
       <c r="A146" s="1" t="s">
         <v>451</v>
       </c>
@@ -4491,7 +4490,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="150" spans="1:5" ht="48" hidden="1">
+    <row r="150" spans="1:5" ht="48">
       <c r="A150" s="1" t="s">
         <v>463</v>
       </c>
@@ -4505,7 +4504,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="151" spans="1:5" ht="80" hidden="1">
+    <row r="151" spans="1:5" ht="80">
       <c r="A151" s="1" t="s">
         <v>466</v>
       </c>
@@ -4877,16 +4876,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E172" xr:uid="{E12BFB51-6AC8-654F-A754-6CA04507B0D4}">
-    <filterColumn colId="4">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-    <sortState ref="A2:E172">
-      <sortCondition sortBy="cellColor" ref="E1:E172" dxfId="0"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>